<commit_message>
solve 2023B quetion1 and question2
</commit_message>
<xml_diff>
--- a/多波束测线问题(2023B)/result1.xlsx
+++ b/多波束测线问题(2023B)/result1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17951" windowHeight="9767"/>
+    <workbookView windowWidth="18288" windowHeight="9767"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>测线距中心点处的距离/m</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>——</t>
-  </si>
-  <si>
-    <t>不重叠</t>
   </si>
 </sst>
 </file>
@@ -1012,13 +1009,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="3"/>
   <cols>
     <col min="1" max="1" width="15.6666666666667" style="2" customWidth="1"/>
     <col min="2" max="8" width="12.8888888888889"/>
@@ -1129,36 +1126,28 @@
         <v>4</v>
       </c>
       <c r="C4" s="4">
-        <v>106.239475042489</v>
+        <v>20.9462103504215</v>
       </c>
       <c r="D4" s="4">
-        <v>88.0537073347435</v>
+        <v>18.0063169822532</v>
       </c>
       <c r="E4" s="4">
-        <v>69.8679396269975</v>
+        <v>14.8393173052909</v>
       </c>
       <c r="F4" s="4">
-        <v>51.6821719192516</v>
+        <v>11.4178381417183</v>
       </c>
       <c r="G4" s="4">
-        <v>33.4964042115057</v>
+        <v>7.70992311478901</v>
       </c>
       <c r="H4" s="4">
-        <v>15.3106365037598</v>
+        <v>3.67803151404114</v>
       </c>
       <c r="I4" s="4">
-        <v>-2.87513120398609</v>
+        <v>0</v>
       </c>
       <c r="J4" s="4">
-        <v>-21.060898911732</v>
-      </c>
-    </row>
-    <row r="5" spans="9:10">
-      <c r="I5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>